<commit_message>
bu lt from my computer
</commit_message>
<xml_diff>
--- a/data/RD/仪表盘-研发组-10-2.xlsx
+++ b/data/RD/仪表盘-研发组-10-2.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="0" windowWidth="18250" windowHeight="7880"/>
+    <workbookView xWindow="3800" yWindow="0" windowWidth="18250" windowHeight="7880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -42,9 +42,6 @@
     <t>封彦杰</t>
   </si>
   <si>
-    <t>蛋白&amp;医学研发组</t>
-  </si>
-  <si>
     <t>10-2</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>任雪</t>
   </si>
   <si>
-    <t>生物学DNA</t>
-  </si>
-  <si>
     <t>刘江</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
   </si>
   <si>
     <t>范旭宁</t>
-  </si>
-  <si>
-    <t>转录调控研发组</t>
   </si>
   <si>
     <t>赵玥</t>
@@ -123,13 +114,22 @@
   <si>
     <t>日期</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生物学DNA组</t>
+  </si>
+  <si>
+    <t>蛋白和医学组</t>
+  </si>
+  <si>
+    <t>转录调控组</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,13 +157,41 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -190,10 +218,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -201,9 +232,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -506,7 +547,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -516,10 +557,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -540,44 +581,44 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="16.5">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="B2" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16.5">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="B3" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -598,15 +639,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="16.5">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -627,15 +668,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="16.5">
       <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -656,15 +697,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="16.5">
       <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>7</v>
@@ -685,15 +726,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="16.5">
       <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -714,15 +755,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="16.5">
       <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -743,15 +784,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="16.5">
       <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -772,15 +813,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="16.5">
       <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
         <v>15</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -801,15 +842,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" ht="16.5">
       <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -830,15 +871,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" ht="16.5">
       <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -859,15 +900,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="16.5">
       <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>7</v>
@@ -890,13 +931,13 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -919,13 +960,13 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -946,15 +987,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="16.5">
       <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -975,15 +1016,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" ht="16.5">
       <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17">
         <v>4</v>
@@ -1004,15 +1045,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" ht="16.5">
       <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1033,15 +1074,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" ht="16.5">
       <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
         <v>25</v>
       </c>
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -1062,15 +1103,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" ht="16.5">
       <c r="A20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -1091,15 +1132,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" ht="14.5">
       <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -1120,15 +1161,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="16.5">
       <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>4</v>

</xml_diff>